<commit_message>
continued ml exploration..almost there
</commit_message>
<xml_diff>
--- a/preprocessing/spotify_training_record.xlsx
+++ b/preprocessing/spotify_training_record.xlsx
@@ -1,39 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JM070903\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Documents/Python/Machine Learning Projects/Spotify_Listening_Analysis/Spotify 2.0/preprocessing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1013053-2FFA-4B76-9352-7F2ED57B3E93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81644EB5-50CA-6440-9A5A-1EB1D9E02829}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29130" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3428EDDC-606B-41BE-B344-5A5E69A49A05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{3428EDDC-606B-41BE-B344-5A5E69A49A05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Number of layers</t>
   </si>
@@ -99,6 +92,78 @@
   </si>
   <si>
     <t xml:space="preserve">Hidden layer no. </t>
+  </si>
+  <si>
+    <t>With outliers</t>
+  </si>
+  <si>
+    <t>Optimizer</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>learning_rate=0.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> beta_1=0.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> beta_2=0.999</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> epsilon=1e-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> amsgrad=False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss </t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Input Activation</t>
+  </si>
+  <si>
+    <t>Output Activation</t>
+  </si>
+  <si>
+    <t>Relu</t>
+  </si>
+  <si>
+    <t>Validation loss is not reducing with more complicated networks</t>
+  </si>
+  <si>
+    <t>Looks like 2 neurons at 50 epochs works well enough</t>
+  </si>
+  <si>
+    <t>Dogs</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>tan</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>dog1</t>
+  </si>
+  <si>
+    <t>dog2</t>
   </si>
 </sst>
 </file>
@@ -468,195 +533,700 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829336AD-A4A9-4D03-91D0-4AE8D7911C7B}">
-  <dimension ref="I5:AC14"/>
+  <dimension ref="B2:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="R5" s="2" t="s">
+    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-    </row>
-    <row r="6" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I6" s="1" t="s">
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1" t="s">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I7">
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E8">
         <v>2</v>
       </c>
-      <c r="J7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K7">
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8">
         <v>25</v>
       </c>
-      <c r="L7">
-        <v>42</v>
-      </c>
-      <c r="Q7" s="1" t="s">
+      <c r="H8">
+        <v>42</v>
+      </c>
+      <c r="I8">
+        <v>1171.96435546875</v>
+      </c>
+      <c r="J8">
+        <v>6.7403335571289</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="R7">
-        <v>50</v>
-      </c>
-      <c r="S7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="9:29" x14ac:dyDescent="0.25">
-      <c r="I8">
+      <c r="N8">
+        <v>50</v>
+      </c>
+      <c r="O8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E9">
         <v>2</v>
       </c>
-      <c r="J8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8">
-        <v>50</v>
-      </c>
-      <c r="L8">
-        <v>42</v>
-      </c>
-      <c r="Q8" s="1"/>
-      <c r="R8">
-        <v>50</v>
-      </c>
-      <c r="S8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <v>50</v>
+      </c>
+      <c r="H9">
+        <v>42</v>
+      </c>
       <c r="I9">
+        <v>6.2431864738464302</v>
+      </c>
+      <c r="J9">
+        <v>6.6333060264587402</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9">
+        <v>50</v>
+      </c>
+      <c r="O9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E10">
         <v>2</v>
       </c>
-      <c r="J9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9">
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10">
         <v>100</v>
       </c>
-      <c r="L9">
-        <v>42</v>
-      </c>
-      <c r="R9">
-        <v>50</v>
-      </c>
-      <c r="S9">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>5.9763503074645996</v>
+      </c>
+      <c r="J10">
+        <v>6.5064620971679599</v>
+      </c>
+      <c r="N10">
+        <v>50</v>
+      </c>
+      <c r="O10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>25</v>
+      </c>
+      <c r="H11">
+        <v>42</v>
+      </c>
+      <c r="I11">
+        <v>7.4949212074279696</v>
+      </c>
+      <c r="J11">
+        <v>6.7087993621826101</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>42</v>
+      </c>
       <c r="I12">
+        <v>956.376220703125</v>
+      </c>
+      <c r="J12">
+        <v>6.6731371879577601</v>
+      </c>
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B13">
         <v>5</v>
       </c>
-      <c r="J12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>42</v>
+      </c>
       <c r="I13">
+        <v>6.3025927543640101</v>
+      </c>
+      <c r="J13">
+        <v>6.4909996986389098</v>
+      </c>
+      <c r="N13">
+        <v>100</v>
+      </c>
+      <c r="O13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B14">
         <v>10</v>
       </c>
-      <c r="J13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="9:29" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <v>25</v>
+      </c>
+      <c r="H14">
+        <v>42</v>
+      </c>
       <c r="I14">
+        <v>6.0578436851501403</v>
+      </c>
+      <c r="J14">
+        <v>6.6946568489074698</v>
+      </c>
+      <c r="N14">
+        <v>50</v>
+      </c>
+      <c r="O14">
+        <v>20</v>
+      </c>
+      <c r="P14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="B15">
         <v>12</v>
       </c>
-      <c r="J14" t="s">
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>42</v>
+      </c>
+      <c r="I15">
+        <v>5.5366916656494096</v>
+      </c>
+      <c r="J15">
+        <v>6.5329561233520499</v>
+      </c>
+      <c r="N15">
+        <v>50</v>
+      </c>
+      <c r="O15">
+        <v>20</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>42</v>
+      </c>
+      <c r="I16">
+        <v>5.0182323455810502</v>
+      </c>
+      <c r="J16">
+        <v>6.0807118415832502</v>
+      </c>
+      <c r="N16">
+        <v>50</v>
+      </c>
+      <c r="O16">
+        <v>20</v>
+      </c>
+      <c r="P16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17">
+        <v>150</v>
+      </c>
+      <c r="H17">
+        <v>42</v>
+      </c>
+      <c r="I17">
+        <v>6.2962040901184002</v>
+      </c>
+      <c r="J17">
+        <v>8.9264974594116193</v>
+      </c>
+      <c r="N17">
+        <v>50</v>
+      </c>
+      <c r="O17">
+        <v>20</v>
+      </c>
+      <c r="P17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
+      </c>
+      <c r="H18">
+        <v>42</v>
+      </c>
+      <c r="I18">
+        <v>6.2962040901184002</v>
+      </c>
+      <c r="J18">
+        <v>4.71262454986572</v>
+      </c>
+      <c r="N18">
+        <v>70</v>
+      </c>
+      <c r="O18">
+        <v>50</v>
+      </c>
+      <c r="P18">
+        <v>30</v>
+      </c>
+      <c r="Q18">
+        <v>20</v>
+      </c>
+      <c r="R18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+      <c r="H19">
+        <v>42</v>
+      </c>
+      <c r="I19">
+        <v>6.2962040901184002</v>
+      </c>
+      <c r="J19">
+        <v>3.36697053909301</v>
+      </c>
+      <c r="N19">
+        <v>70</v>
+      </c>
+      <c r="O19">
+        <v>50</v>
+      </c>
+      <c r="P19">
+        <v>30</v>
+      </c>
+      <c r="Q19">
+        <v>20</v>
+      </c>
+      <c r="R19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23">
+        <v>50</v>
+      </c>
+      <c r="H23">
+        <v>42</v>
+      </c>
+      <c r="I23">
+        <v>6.2962040901184002</v>
+      </c>
+      <c r="J23">
+        <v>4.71262454986572</v>
+      </c>
+      <c r="N23">
+        <v>50</v>
+      </c>
+      <c r="O23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="H24">
+        <v>42</v>
+      </c>
+      <c r="I24">
+        <v>6.2962040901184002</v>
+      </c>
+      <c r="J24">
+        <v>3.36697053909301</v>
+      </c>
+      <c r="N24">
+        <v>50</v>
+      </c>
+      <c r="O24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="5:18" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <v>50</v>
+      </c>
+      <c r="H28">
+        <v>10</v>
+      </c>
+      <c r="I28">
+        <v>6.2962040901184002</v>
+      </c>
+      <c r="J28">
+        <v>4.71262454986572</v>
+      </c>
+      <c r="N28">
+        <v>50</v>
+      </c>
+      <c r="O28">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="R5:AC5"/>
+    <mergeCell ref="N6:Y6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72254E17-DD31-1B4B-8433-8BE0BDE9E865}">
+  <dimension ref="D5:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="5" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>